<commit_message>
Manual Testing Classwork Excel File
</commit_message>
<xml_diff>
--- a/Manual Testing Classwork.xlsx
+++ b/Manual Testing Classwork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAFFDC4-84F8-4579-BFB8-0B571C44F085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E8A7AE-A7CA-46B8-9F26-997D94282018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4251631F-0E37-4D4E-916C-A530EB300A89}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Project Name:</t>
   </si>
@@ -157,6 +157,63 @@
   </si>
   <si>
     <t>No Comments</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_002</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_003</t>
+  </si>
+  <si>
+    <t>TC_ERP_Login_004</t>
+  </si>
+  <si>
+    <t>Enter a valid user name &amp; an invalid password</t>
+  </si>
+  <si>
+    <t>Enter an invalid user name &amp; a valid password</t>
+  </si>
+  <si>
+    <t>Enter an invalid user name &amp; an invalid password</t>
+  </si>
+  <si>
+    <t>1. Enter valid username
+2. Enter invalid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter valid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>1. Enter invalid username
+2. Enter invalid password
+3. Click on the login button</t>
+  </si>
+  <si>
+    <t>Username: admin@erp.com
+Password:
+xxxx</t>
+  </si>
+  <si>
+    <t>Username: xxxx@erp.com
+Password:
+xxxx</t>
+  </si>
+  <si>
+    <t>Username: xxxx@erp.com
+Password:
+P@ssw0rd</t>
+  </si>
+  <si>
+    <t>Still remaining on the login Page</t>
+  </si>
+  <si>
+    <t>Unsuccessful Login</t>
+  </si>
+  <si>
+    <t>A popup message box to show an error message "Invalid Username/Password"</t>
   </si>
 </sst>
 </file>
@@ -166,7 +223,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="dd/mmm/yyyy\ \(ddd\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -198,8 +255,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,8 +281,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -431,11 +512,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -458,50 +578,71 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,9 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD3C831-BEC5-49D4-824C-4957A756F525}">
   <dimension ref="A2:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -849,10 +988,10 @@
     <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
@@ -916,144 +1055,229 @@
     </row>
     <row r="9" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:14" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="12" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="13">
         <v>45362</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="21"/>
+    <row r="12" spans="1:14" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="24">
+        <v>45362</v>
+      </c>
+      <c r="N12" s="25" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="21"/>
+    <row r="13" spans="1:14" s="2" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="13">
+        <v>45363</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="24"/>
+    <row r="14" spans="1:14" s="2" customFormat="1" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="30">
+        <v>45363</v>
+      </c>
+      <c r="N14" s="31" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>